<commit_message>
project update and result
</commit_message>
<xml_diff>
--- a/TesProject/src/main/resource/data_provider_sheet.xlsx
+++ b/TesProject/src/main/resource/data_provider_sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vn0jp2r/git_repos/dev_zuber_2020/asda_search_RestAssuredPOC/schema_valiadator/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vn06185/Documents/Personal/TesProject/src/main/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBC481E-320A-534C-945D-9111C8D85222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDB374D-2697-8744-B31D-00F210729338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="2400" windowWidth="26440" windowHeight="14220" xr2:uid="{7E39010B-5DFC-6244-B29D-D9968E5C6475}"/>
   </bookViews>
@@ -33,9 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>URLS</t>
+  </si>
+  <si>
+    <t>https://bit.ly/2MMhOhs</t>
   </si>
   <si>
     <t>https://bit.ly/2sDY4pl</t>
@@ -84,27 +87,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -127,37 +115,16 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -467,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77B4277-1F38-2747-87AC-8767A75A946D}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -488,13 +455,15 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1" stopIfTrue="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2" stopIfTrue="1"/>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6AC0BE8F-9A4A-4D45-A020-8A0419A03808}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E6092AB4-F72B-824B-93C2-DE13B72C7850}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{EABFDDE1-8F95-C248-BF5B-C444B6B9EB99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>